<commit_message>
add calendar bug ver & fix triangle bug
</commit_message>
<xml_diff>
--- a/src/main/resources/commissionTestCases.xlsx
+++ b/src/main/resources/commissionTestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20359"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\github\testPractice\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92A832D-7CA8-4275-AFAF-C3DC47D4D132}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1DFB97-BC25-47E2-B7E7-83D504E0D89C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>测试用例编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,63 +107,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>650.0</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
-  <si>
-    <t>655.0</t>
-  </si>
-  <si>
-    <t>990.0</t>
-  </si>
-  <si>
-    <t>995.0</t>
-  </si>
-  <si>
-    <t>586.0</t>
-  </si>
-  <si>
-    <t>592.0</t>
-  </si>
-  <si>
-    <t>1054.0</t>
-  </si>
-  <si>
-    <t>424.0</t>
-  </si>
-  <si>
-    <t>433.0</t>
-  </si>
-  <si>
-    <t>1216.0</t>
-  </si>
-  <si>
-    <t>1225.0</t>
-  </si>
-  <si>
-    <t>820.0</t>
-  </si>
-  <si>
-    <t>1060.0</t>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.0</t>
-  </si>
-  <si>
-    <t>fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,12 +437,12 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" style="1" width="9.0" collapsed="true"/>
+    <col min="5" max="5" width="9" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -533,12 +484,6 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -556,12 +501,6 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -579,12 +518,6 @@
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -602,12 +535,6 @@
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -625,12 +552,6 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -648,12 +569,6 @@
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -671,12 +586,6 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -694,12 +603,6 @@
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -717,12 +620,6 @@
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -740,12 +637,6 @@
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -763,12 +654,6 @@
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -786,12 +671,6 @@
       <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -809,12 +688,6 @@
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -830,13 +703,7 @@
         <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>